<commit_message>
Bait Type Effect and PERMANOVA
</commit_message>
<xml_diff>
--- a/SIMPER_data_withoutsharks.xlsx
+++ b/SIMPER_data_withoutsharks.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\17193\Downloads\salvador\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D01EFB47-6288-41BF-9085-7A9E2F833640}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB2F7DC8-9C06-4BE7-8A9D-90EEFD32AD7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{A8595ED7-EDA5-4240-89F7-67B129589F6D}"/>
   </bookViews>

</xml_diff>